<commit_message>
Add prefix to 10
</commit_message>
<xml_diff>
--- a/Wiki_Ava.xlsx
+++ b/Wiki_Ava.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Surface</t>
   </si>
@@ -91,7 +91,7 @@
     </r>
   </si>
   <si>
-    <t> Methodist Ladies ' College</t>
+    <t>Methodist Ladies ' College</t>
   </si>
   <si>
     <t>53715bd0a310958a4e6ade79</t>
@@ -196,6 +196,101 @@
   </si>
   <si>
     <t>Calvert</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6adeb3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Charles_Calvert,_5th_Baron_Baltimore</t>
+    </r>
+  </si>
+  <si>
+    <t>Baron_Baltimore</t>
+  </si>
+  <si>
+    <t>Maccabi Haifa</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6adeb8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maccabi_Haifa_B.C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Maccabi_Haifa_F.C.</t>
+  </si>
+  <si>
+    <t>British</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6adec4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">United_Kingdom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Presidencies_and_provinces_of…</t>
+  </si>
+  <si>
+    <t>triads</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6aded9</t>
+  </si>
+  <si>
+    <t>Triad_(music)</t>
+  </si>
+  <si>
+    <t>Chord_(music)</t>
+  </si>
+  <si>
+    <t>Miesbach</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6adee9</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Miesbach_(district)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -317,14 +412,14 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0765306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0765306122449"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6734693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
@@ -464,9 +559,87 @@
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11"/>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14"/>
   </sheetData>
@@ -486,6 +659,21 @@
     <hyperlink display="Republic" ref="C6" r:id="rId13"/>
     <hyperlink display="The_Republic_(Plato)" ref="D6" r:id="rId14"/>
     <hyperlink display="link" ref="E6" r:id="rId15"/>
+    <hyperlink display="Charles_Calvert,_5th_Baron_Baltimore" ref="C7" r:id="rId16"/>
+    <hyperlink display="Baron_Baltimore" ref="D7" r:id="rId17"/>
+    <hyperlink display="link" ref="E7" r:id="rId18"/>
+    <hyperlink display="Maccabi_Haifa_B.C." ref="C8" r:id="rId19"/>
+    <hyperlink display="Maccabi_Haifa_F.C." ref="D8" r:id="rId20"/>
+    <hyperlink display="link" ref="E8" r:id="rId21"/>
+    <hyperlink display="United_Kingdom" ref="C9" r:id="rId22"/>
+    <hyperlink display="Presidencies_and_provinces_of…" ref="D9" r:id="rId23"/>
+    <hyperlink display="link" ref="E9" r:id="rId24"/>
+    <hyperlink display="Triad_(music)" ref="C10" r:id="rId25"/>
+    <hyperlink display="Chord_(music)" ref="D10" r:id="rId26"/>
+    <hyperlink display="link" ref="E10" r:id="rId27"/>
+    <hyperlink display="Miesbach_(district)" ref="C11" r:id="rId28"/>
+    <hyperlink display="Miesbach" ref="D11" r:id="rId29"/>
+    <hyperlink display="link" ref="E11" r:id="rId30"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add prefix to 11
</commit_message>
<xml_diff>
--- a/Wiki_Ava.xlsx
+++ b/Wiki_Ava.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Surface</t>
   </si>
@@ -291,6 +291,29 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>Portland Timbers</t>
+  </si>
+  <si>
+    <t>53715bd0a310958a4e6adef8</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Portland_Timbers_(USL)</t>
+    </r>
+  </si>
+  <si>
+    <t>Portland_Timbers</t>
   </si>
 </sst>
 </file>
@@ -412,7 +435,7 @@
   <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
+      <selection activeCell="D12" activeCellId="0" pane="topLeft" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -638,6 +661,23 @@
       </c>
       <c r="E11" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="12">
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13"/>
@@ -674,6 +714,9 @@
     <hyperlink display="Miesbach_(district)" ref="C11" r:id="rId28"/>
     <hyperlink display="Miesbach" ref="D11" r:id="rId29"/>
     <hyperlink display="link" ref="E11" r:id="rId30"/>
+    <hyperlink display="Portland_Timbers_(USL)" ref="C12" r:id="rId31"/>
+    <hyperlink display="Portland_Timbers" ref="D12" r:id="rId32"/>
+    <hyperlink display="link" ref="E12" r:id="rId33"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>